<commit_message>
Updated readme correct worksheet name
</commit_message>
<xml_diff>
--- a/excel_helpers/WEBCON BPS Helpers.xlsx
+++ b/excel_helpers/WEBCON BPS Helpers.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cosmo365.sharepoint.com/sites/cosmols_rnd/Shared Documents/Drafts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\_Privat\private_github\webcon_helpers\excel_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3D4B218-5C87-47AD-BB04-837C5729FE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C9359E-5004-4406-8A68-114F7FFBC735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="345" windowWidth="23865" windowHeight="12975" activeTab="2" xr2:uid="{515E2740-26BF-40E8-9847-8123C6783471}"/>
+    <workbookView xWindow="30510" yWindow="1695" windowWidth="23865" windowHeight="12975" activeTab="1" xr2:uid="{515E2740-26BF-40E8-9847-8123C6783471}"/>
   </bookViews>
   <sheets>
     <sheet name="Choice field" sheetId="1" r:id="rId1"/>
-    <sheet name="User specific label" sheetId="2" r:id="rId2"/>
+    <sheet name="Multilingual icon" sheetId="2" r:id="rId2"/>
     <sheet name="SQL Command templates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Define labels for the necessary languages in row 10</t>
-  </si>
-  <si>
-    <t>Copy case statement below the table in A14</t>
   </si>
   <si>
     <t>Set the Ids of the values, if you don't use constants</t>
@@ -279,6 +276,9 @@
 where DET_WFDID = WORKFLOWID
   and DET_WFCONID = ITEMLISTFIELDID
   and WFD_COMID = {COM_ID}</t>
+  </si>
+  <si>
+    <t>Copy case statement below the table in A16</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BADBE0-67ED-490A-B3C4-B6F30EF8991B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1014,12 +1014,12 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1130,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CA6BB9-7F40-4A1C-97A7-1F0A93A9537F}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="2" spans="1:1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1156,7 +1156,7 @@
     </row>
     <row r="4" spans="1:1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -1166,7 +1166,7 @@
     </row>
     <row r="6" spans="1:1" ht="90.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
@@ -1191,12 +1191,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="137.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1206,6 +1206,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001710DCA9406EC4409CAF62CAB2EEC7CB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1314eb49a0e74ce23cbca31ec97881f1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52b7af4b-4865-43e8-ac17-ae48558bfc23" xmlns:ns3="b0825c7e-e9c2-4b89-b254-acd72817bce9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="479cd2957f1d1463cde28b59774d65f9" ns2:_="" ns3:_="">
     <xsd:import namespace="52b7af4b-4865-43e8-ac17-ae48558bfc23"/>
@@ -1416,36 +1431,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07423078-AA80-4983-A346-0FEBA77414F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD74555A-5BFB-4545-A1B7-C75CAAE39BBB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="52b7af4b-4865-43e8-ac17-ae48558bfc23"/>
-    <ds:schemaRef ds:uri="b0825c7e-e9c2-4b89-b254-acd72817bce9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1468,9 +1457,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD74555A-5BFB-4545-A1B7-C75CAAE39BBB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07423078-AA80-4983-A346-0FEBA77414F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="52b7af4b-4865-43e8-ac17-ae48558bfc23"/>
+    <ds:schemaRef ds:uri="b0825c7e-e9c2-4b89-b254-acd72817bce9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>